<commit_message>
Added status information and removed h5 dependency
</commit_message>
<xml_diff>
--- a/constructor compare.xlsx
+++ b/constructor compare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://actondatanl-my.sharepoint.com/personal/eric_ruis_actondata_nl/Documents/Projecten/Smartbox/nodes/node-red-contrib-machine-learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{0885D2C0-DFE1-40BA-9171-F426832158D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7680CC9C-9043-4AD2-BA6F-CD58B4925A4E}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="8_{0885D2C0-DFE1-40BA-9171-F426832158D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8932B142-6831-4C7B-B468-804F06CD9573}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="33946" windowHeight="21975" xr2:uid="{5E62D054-A6B8-4176-9CF5-8B96DE512F6E}"/>
+    <workbookView xWindow="2040" yWindow="2753" windowWidth="21667" windowHeight="15675" xr2:uid="{5E62D054-A6B8-4176-9CF5-8B96DE512F6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Regressor" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="64">
   <si>
     <t>Random forest</t>
   </si>
@@ -209,6 +209,24 @@
   </si>
   <si>
     <t>max_fun</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>tuple</t>
+  </si>
+  <si>
+    <t>int/bool</t>
   </si>
 </sst>
 </file>
@@ -269,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -283,6 +301,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46318ADB-2A60-437C-8165-201AFE7AD98C}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -612,6 +636,7 @@
     <col min="4" max="4" width="12.9296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.46484375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.06640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" ht="86.25" x14ac:dyDescent="0.45">
@@ -631,6 +656,7 @@
       <c r="F1" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
@@ -639,6 +665,9 @@
       <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G2" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -655,6 +684,9 @@
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G4" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
@@ -663,6 +695,9 @@
       <c r="F5" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G5" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
@@ -671,6 +706,9 @@
       <c r="F6" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G6" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
@@ -679,6 +717,9 @@
       <c r="F7" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G7" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
@@ -687,7 +728,9 @@
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="7" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
@@ -696,6 +739,9 @@
       <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G9" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
@@ -704,6 +750,9 @@
       <c r="D10" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G10" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
@@ -715,6 +764,9 @@
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G11" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
@@ -723,6 +775,9 @@
       <c r="D12" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G12" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
@@ -734,6 +789,9 @@
       <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G13" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
@@ -742,6 +800,9 @@
       <c r="D14" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G14" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
@@ -750,6 +811,9 @@
       <c r="F15" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G15" s="7" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
@@ -761,24 +825,33 @@
       <c r="F16" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G16" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G17" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G18" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -786,7 +859,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -794,23 +867,29 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G21" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G22" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -820,8 +899,11 @@
       <c r="C23" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G23" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -831,308 +913,385 @@
       <c r="C24" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G24" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G27" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A46" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A47" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A49" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A52" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A53" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B54" s="1">
+        <f>COUNTIF(B2:B53,"x")</f>
         <v>17</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="2" t="s">
+      <c r="C54" s="1">
+        <f>COUNTIF(C2:C53,"x")</f>
         <v>11</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A49" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A50" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A51" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A52" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A53" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A54" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B55" s="1">
-        <f>COUNTIF(B2:B54,"x")</f>
-        <v>17</v>
-      </c>
-      <c r="C55" s="1">
-        <f>COUNTIF(C2:C54,"x")</f>
+      <c r="D54" s="1">
+        <f t="shared" ref="D54:F54" si="0">COUNTIF(D2:D53,"x")</f>
         <v>11</v>
       </c>
-      <c r="D55" s="1">
-        <f t="shared" ref="D55:F55" si="0">COUNTIF(D2:D54,"x")</f>
-        <v>11</v>
-      </c>
-      <c r="E55" s="1">
+      <c r="E54" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F54" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
+      <c r="G54" s="7">
+        <f>COUNTA(G2:G53)</f>
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F53">
-    <sortCondition ref="A2:A53"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F52">
+    <sortCondition ref="A2:A52"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>